<commit_message>
Control de Documentos JCSGC
</commit_message>
<xml_diff>
--- a/-nuevoRD.xlsx
+++ b/-nuevoRD.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
   <si>
     <t xml:space="preserve">           CONDICIONES DE TRABAJO, INSPECCION Y COMENTARIOS PARA PIEZAS LIBERADAS</t>
   </si>
@@ -135,7 +135,7 @@
     <t xml:space="preserve">      RETENCION DIMENSIONAL DE REGISTROS DE CALIDAD</t>
   </si>
   <si>
-    <t>19/01/2024</t>
+    <t>01/02/2024</t>
   </si>
   <si>
     <t>BF - 384 - 23</t>
@@ -144,82 +144,28 @@
     <t>OK</t>
   </si>
   <si>
-    <t>PRUEBA</t>
+    <t>INSPECCIÓN 100%</t>
   </si>
   <si>
     <t>02/02/2024</t>
   </si>
   <si>
-    <t>INSPECCIÓN 100%</t>
+    <t>07/06/2024</t>
   </si>
   <si>
-    <t>130359 </t>
+    <t>11/06/2024</t>
   </si>
   <si>
-    <t>55057475</t>
+    <t>110001</t>
   </si>
   <si>
-    <t>2458</t>
+    <t>1345</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>DIÁMETRO EXT.
-1.821 - 1.825</t>
-  </si>
-  <si>
-    <t>DIÁMETRO DE BARRENO
-0.9605 - 0.9685</t>
-  </si>
-  <si>
-    <t>CONCENTRICIDAD
-0.008</t>
-  </si>
-  <si>
-    <t>ESPESOR BASE
-0.094 - 0.120</t>
-  </si>
-  <si>
-    <t>CONCAVIDAD
-0.010 MAX</t>
-  </si>
-  <si>
-    <t>PLANICIDAD
-0.003</t>
-  </si>
-  <si>
-    <t>1.822</t>
-  </si>
-  <si>
-    <t>0.966</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>0.100</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>P201286</t>
-  </si>
-  <si>
-    <t>16000</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
 </sst>
 </file>
@@ -229,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -324,38 +270,6 @@
       <name val="Calibri"/>
       <sz val="7.0"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="6.0"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -371,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -991,26 +905,11 @@
         <color indexed="8"/>
       </top>
     </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
@@ -1347,84 +1246,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="0" applyFont="true" applyBorder="true">
       <alignment textRotation="90" wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2412,7 +2233,7 @@
       <c r="O8" s="50"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R8" s="50"/>
       <c r="S8" s="50"/>
@@ -2446,20 +2267,28 @@
       <c r="C9" s="29">
         <v>3</v>
       </c>
-      <c r="D9" s="53"/>
+      <c r="D9" s="53" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
       <c r="H9" s="26"/>
-      <c r="I9" s="50"/>
+      <c r="I9" s="50" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="50"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="50"/>
+      <c r="L9" s="50" t="s">
+        <v>35</v>
+      </c>
       <c r="M9" s="50"/>
       <c r="N9" s="50"/>
       <c r="O9" s="50"/>
       <c r="P9" s="26"/>
-      <c r="Q9" s="50"/>
+      <c r="Q9" s="50" t="s">
+        <v>36</v>
+      </c>
       <c r="R9" s="50"/>
       <c r="S9" s="50"/>
       <c r="T9" s="50"/>
@@ -2492,20 +2321,28 @@
       <c r="C10" s="29">
         <v>4</v>
       </c>
-      <c r="D10" s="53"/>
+      <c r="D10" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
       <c r="G10" s="50"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="50"/>
+      <c r="I10" s="50" t="s">
+        <v>34</v>
+      </c>
       <c r="J10" s="50"/>
       <c r="K10" s="26"/>
-      <c r="L10" s="50"/>
+      <c r="L10" s="50" t="s">
+        <v>35</v>
+      </c>
       <c r="M10" s="50"/>
       <c r="N10" s="50"/>
       <c r="O10" s="50"/>
       <c r="P10" s="26"/>
-      <c r="Q10" s="50"/>
+      <c r="Q10" s="50" t="s">
+        <v>36</v>
+      </c>
       <c r="R10" s="50"/>
       <c r="S10" s="50"/>
       <c r="T10" s="50"/>
@@ -5911,7 +5748,7 @@
       <c r="L3" s="95"/>
       <c r="M3" s="95"/>
       <c r="N3" s="80" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O3" s="80"/>
       <c r="P3" s="80"/>
@@ -5922,7 +5759,7 @@
       <c r="S3" s="81"/>
       <c r="T3" s="81"/>
       <c r="U3" s="80" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V3" s="80"/>
       <c r="W3" s="80"/>
@@ -5932,7 +5769,7 @@
       <c r="Y3" s="81"/>
       <c r="Z3" s="81"/>
       <c r="AA3" s="80" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB3" s="80"/>
       <c r="AC3" s="80"/>
@@ -5990,14 +5827,16 @@
         <v>18</v>
       </c>
       <c r="M5" s="83" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N5" s="84"/>
       <c r="O5" s="5"/>
       <c r="P5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="82"/>
+      <c r="Q5" s="82" t="s">
+        <v>43</v>
+      </c>
       <c r="R5" s="82"/>
       <c r="S5" s="2"/>
       <c r="T5" s="11" t="s">
@@ -6030,29 +5869,17 @@
       <c r="G6" s="105"/>
       <c r="H6" s="106"/>
       <c r="I6" s="96"/>
-      <c r="J6" s="64" t="s">
-        <v>44</v>
-      </c>
+      <c r="J6" s="64"/>
       <c r="K6" s="74"/>
-      <c r="L6" s="64" t="s">
-        <v>45</v>
-      </c>
+      <c r="L6" s="64"/>
       <c r="M6" s="74"/>
-      <c r="N6" s="64" t="s">
-        <v>46</v>
-      </c>
+      <c r="N6" s="64"/>
       <c r="O6" s="71"/>
-      <c r="P6" s="64" t="s">
-        <v>47</v>
-      </c>
+      <c r="P6" s="64"/>
       <c r="Q6" s="71"/>
-      <c r="R6" s="64" t="s">
-        <v>48</v>
-      </c>
+      <c r="R6" s="64"/>
       <c r="S6" s="74"/>
-      <c r="T6" s="64" t="s">
-        <v>49</v>
-      </c>
+      <c r="T6" s="64"/>
       <c r="U6" s="74"/>
       <c r="V6" s="64"/>
       <c r="W6" s="74"/>
@@ -6177,54 +6004,28 @@
       <c r="AD9" s="66"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="153" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="154" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="155" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="156" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="157" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="158" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="160" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="136" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="137"/>
-      <c r="K10" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="140"/>
-      <c r="M10" s="142" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="143"/>
-      <c r="O10" s="145" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="146"/>
-      <c r="Q10" s="148" t="s">
-        <v>52</v>
-      </c>
-      <c r="R10" s="149"/>
-      <c r="S10" s="151" t="s">
-        <v>52</v>
-      </c>
-      <c r="T10" s="152"/>
+      <c r="A10" s="44">
+        <v>1</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
       <c r="U10" s="79"/>
       <c r="V10" s="79"/>
       <c r="W10" s="79"/>
@@ -7273,7 +7074,7 @@
       <c r="L41" s="95"/>
       <c r="M41" s="95"/>
       <c r="N41" s="80" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O41" s="80"/>
       <c r="P41" s="80"/>
@@ -7284,7 +7085,7 @@
       <c r="S41" s="81"/>
       <c r="T41" s="81"/>
       <c r="U41" s="80" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V41" s="80"/>
       <c r="W41" s="80"/>
@@ -7294,7 +7095,7 @@
       <c r="Y41" s="81"/>
       <c r="Z41" s="81"/>
       <c r="AA41" s="80" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB41" s="80"/>
       <c r="AC41" s="80"/>
@@ -7350,14 +7151,16 @@
         <v>18</v>
       </c>
       <c r="M43" s="83" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N43" s="84"/>
       <c r="O43" s="5"/>
       <c r="P43" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q43" s="82"/>
+      <c r="Q43" s="82" t="s">
+        <v>43</v>
+      </c>
       <c r="R43" s="82"/>
       <c r="S43" s="2"/>
       <c r="T43" s="11" t="s">
@@ -8595,7 +8398,7 @@
       <c r="L79" s="95"/>
       <c r="M79" s="95"/>
       <c r="N79" s="80" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O79" s="80"/>
       <c r="P79" s="80"/>
@@ -8606,7 +8409,7 @@
       <c r="S79" s="81"/>
       <c r="T79" s="81"/>
       <c r="U79" s="80" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V79" s="80"/>
       <c r="W79" s="80"/>
@@ -8616,7 +8419,7 @@
       <c r="Y79" s="81"/>
       <c r="Z79" s="81"/>
       <c r="AA79" s="80" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB79" s="80"/>
       <c r="AC79" s="80"/>
@@ -8672,14 +8475,16 @@
         <v>18</v>
       </c>
       <c r="M81" s="83" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N81" s="84"/>
       <c r="O81" s="5"/>
       <c r="P81" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q81" s="82"/>
+      <c r="Q81" s="82" t="s">
+        <v>43</v>
+      </c>
       <c r="R81" s="82"/>
       <c r="S81" s="2"/>
       <c r="T81" s="11" t="s">
@@ -9885,7 +9690,7 @@
       <c r="L117" s="95"/>
       <c r="M117" s="95"/>
       <c r="N117" s="80" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O117" s="80"/>
       <c r="P117" s="80"/>
@@ -9896,7 +9701,7 @@
       <c r="S117" s="81"/>
       <c r="T117" s="81"/>
       <c r="U117" s="80" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V117" s="80"/>
       <c r="W117" s="80"/>
@@ -9906,7 +9711,7 @@
       <c r="Y117" s="81"/>
       <c r="Z117" s="81"/>
       <c r="AA117" s="80" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AB117" s="80"/>
       <c r="AC117" s="80"/>
@@ -9962,14 +9767,16 @@
         <v>18</v>
       </c>
       <c r="M119" s="83" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N119" s="84"/>
       <c r="O119" s="5"/>
       <c r="P119" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Q119" s="82"/>
+      <c r="Q119" s="82" t="s">
+        <v>43</v>
+      </c>
       <c r="R119" s="82"/>
       <c r="S119" s="2"/>
       <c r="T119" s="11" t="s">
@@ -12530,12 +12337,6 @@
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W24:X24"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AI10:AJ10"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AM10:AN10"/>
-    <mergeCell ref="AO10:AP10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1" gridLines="1"/>
   <pageMargins left="0.39370078740157" right="0.51181102362205" top="0.27559055118109999" bottom="0.39370078740157" header="0" footer="0"/>

</xml_diff>